<commit_message>
code fixes and configurable using.env file.
</commit_message>
<xml_diff>
--- a/ai-tsr-crewai/data/tc_execution_report.xlsx
+++ b/ai-tsr-crewai/data/tc_execution_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashish/Documents/GitHub/AiAssistedTestReportGeneration/ai-tsr-crewai/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F459E0-196D-8243-BF50-CA2E6FF6876A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDA11E5-24A2-A640-8B23-F680B2D076D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{DBE6A3A0-94B0-074B-A854-E58D3738C668}"/>
   </bookViews>
@@ -1093,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500B0826-BDED-8C4B-820B-BA9B03BB1156}">
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17:R17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1884,7 +1884,7 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="H17" s="1">
         <v>45909.416666666664</v>

</xml_diff>

<commit_message>
Fixed Priority to Severity Mapping for Quality Gates
</commit_message>
<xml_diff>
--- a/ai-tsr-crewai/data/tc_execution_report.xlsx
+++ b/ai-tsr-crewai/data/tc_execution_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashish/Documents/GitHub/AiAssistedTestReportGeneration/ai-tsr-crewai/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDA11E5-24A2-A640-8B23-F680B2D076D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B5811E-E3B0-8449-BD07-0A5135560AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{DBE6A3A0-94B0-074B-A854-E58D3738C668}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="69">
   <si>
     <t>Module</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Root Cause</t>
   </si>
   <si>
-    <t>Severity</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
@@ -184,9 +181,6 @@
     <t>Low</t>
   </si>
   <si>
-    <t>Minor</t>
-  </si>
-  <si>
     <t>TC003</t>
   </si>
   <si>
@@ -230,6 +224,9 @@
   </si>
   <si>
     <t>Closed</t>
+  </si>
+  <si>
+    <t>Highest</t>
   </si>
 </sst>
 </file>
@@ -1091,10 +1088,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500B0826-BDED-8C4B-820B-BA9B03BB1156}">
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1109,7 +1106,7 @@
     <col min="17" max="17" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1161,710 +1158,689 @@
       <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H2" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s">
         <v>22</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>24</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>25</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>26</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
         <v>27</v>
       </c>
-      <c r="O2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>29</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
         <v>30</v>
       </c>
-      <c r="F3" t="s">
-        <v>31</v>
-      </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
         <v>22</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>23</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>24</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>25</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>26</v>
       </c>
-      <c r="N3" t="s">
-        <v>27</v>
-      </c>
       <c r="O3">
         <v>20</v>
       </c>
       <c r="P3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q3" t="s">
         <v>32</v>
       </c>
-      <c r="Q3" t="s">
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>33</v>
       </c>
-      <c r="R3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>34</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>35</v>
-      </c>
-      <c r="C4" t="s">
-        <v>36</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
         <v>37</v>
-      </c>
-      <c r="G4" t="s">
-        <v>38</v>
       </c>
       <c r="H4" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
         <v>22</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>23</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>24</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>25</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>26</v>
       </c>
-      <c r="N4" t="s">
-        <v>27</v>
-      </c>
       <c r="O4">
         <v>20</v>
       </c>
       <c r="P4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q4" t="s">
-        <v>39</v>
-      </c>
-      <c r="R4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
         <v>34</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>35</v>
-      </c>
-      <c r="C5" t="s">
-        <v>36</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H5" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" t="s">
         <v>22</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>23</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>24</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>25</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>26</v>
       </c>
-      <c r="N5" t="s">
-        <v>27</v>
-      </c>
       <c r="O5">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
         <v>40</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>41</v>
-      </c>
-      <c r="C6" t="s">
-        <v>42</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G6" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="H6" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" t="s">
         <v>22</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>23</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>24</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>25</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>26</v>
       </c>
-      <c r="N6" t="s">
-        <v>27</v>
-      </c>
       <c r="O6">
         <v>20</v>
       </c>
       <c r="P6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
         <v>44</v>
       </c>
-      <c r="R6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>45</v>
-      </c>
-      <c r="C7" t="s">
-        <v>46</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" t="s">
         <v>22</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>23</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>24</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>25</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>26</v>
       </c>
-      <c r="N7" t="s">
-        <v>27</v>
-      </c>
       <c r="O7">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
         <v>47</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>48</v>
-      </c>
-      <c r="C8" t="s">
-        <v>49</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H8" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" t="s">
         <v>22</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>23</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>24</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>25</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>26</v>
       </c>
-      <c r="N8" t="s">
-        <v>27</v>
-      </c>
       <c r="O8">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
         <v>50</v>
-      </c>
-      <c r="C9" t="s">
-        <v>51</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" t="s">
         <v>52</v>
-      </c>
-      <c r="G9" t="s">
-        <v>53</v>
       </c>
       <c r="H9" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" t="s">
         <v>22</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>23</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>24</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>25</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>26</v>
       </c>
-      <c r="N9" t="s">
-        <v>27</v>
-      </c>
       <c r="O9">
         <v>20</v>
       </c>
       <c r="P9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q9" t="s">
-        <v>33</v>
-      </c>
-      <c r="R9" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H10" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" t="s">
         <v>22</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>23</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>24</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>25</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>26</v>
       </c>
-      <c r="N10" t="s">
-        <v>27</v>
-      </c>
       <c r="O10">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H11" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" t="s">
         <v>22</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>23</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>24</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>25</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>26</v>
       </c>
-      <c r="N11" t="s">
-        <v>27</v>
-      </c>
       <c r="O11">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H12" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" t="s">
         <v>22</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>23</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>24</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>25</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>26</v>
       </c>
-      <c r="N12" t="s">
-        <v>27</v>
-      </c>
       <c r="O12">
         <v>20</v>
       </c>
       <c r="P12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q12" t="s">
-        <v>39</v>
-      </c>
-      <c r="R12" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13">
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H13" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" t="s">
         <v>22</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>23</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>24</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>25</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>26</v>
       </c>
-      <c r="N13" t="s">
-        <v>27</v>
-      </c>
       <c r="O13">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H14" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" t="s">
         <v>22</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>23</v>
       </c>
-      <c r="K14" t="s">
-        <v>24</v>
-      </c>
       <c r="L14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M14" t="s">
+        <v>25</v>
+      </c>
+      <c r="N14" t="s">
         <v>26</v>
       </c>
-      <c r="N14" t="s">
-        <v>27</v>
-      </c>
       <c r="O14">
         <v>20</v>
       </c>
       <c r="P14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Q14" t="s">
-        <v>44</v>
-      </c>
-      <c r="R14" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H15" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" t="s">
         <v>22</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>23</v>
       </c>
-      <c r="K15" t="s">
-        <v>24</v>
-      </c>
       <c r="L15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M15" t="s">
+        <v>25</v>
+      </c>
+      <c r="N15" t="s">
         <v>26</v>
       </c>
-      <c r="N15" t="s">
-        <v>27</v>
-      </c>
       <c r="O15">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H16" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16" t="s">
         <v>22</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>23</v>
       </c>
-      <c r="K16" t="s">
-        <v>24</v>
-      </c>
       <c r="L16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M16" t="s">
+        <v>25</v>
+      </c>
+      <c r="N16" t="s">
         <v>26</v>
-      </c>
-      <c r="N16" t="s">
-        <v>27</v>
       </c>
       <c r="O16">
         <v>20</v>
@@ -1872,40 +1848,40 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" t="s">
         <v>65</v>
-      </c>
-      <c r="B17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" t="s">
-        <v>67</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H17" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" t="s">
         <v>22</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>23</v>
       </c>
-      <c r="K17" t="s">
-        <v>24</v>
-      </c>
       <c r="L17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M17" t="s">
+        <v>25</v>
+      </c>
+      <c r="N17" t="s">
         <v>26</v>
-      </c>
-      <c r="N17" t="s">
-        <v>27</v>
       </c>
       <c r="O17">
         <v>20</v>
@@ -1913,5 +1889,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
made agent run with different reports with severity value changes.
</commit_message>
<xml_diff>
--- a/ai-tsr-crewai/data/tc_execution_report.xlsx
+++ b/ai-tsr-crewai/data/tc_execution_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashish/Documents/GitHub/AiAssistedTestReportGeneration/ai-tsr-crewai/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B5811E-E3B0-8449-BD07-0A5135560AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7E299F-1C12-D44A-B0A3-E43E215194BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16380" xr2:uid="{DBE6A3A0-94B0-074B-A854-E58D3738C668}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="73">
   <si>
     <t>Module</t>
   </si>
@@ -73,6 +73,9 @@
     <t>Root Cause</t>
   </si>
   <si>
+    <t>Severity</t>
+  </si>
+  <si>
     <t>Login</t>
   </si>
   <si>
@@ -181,6 +184,9 @@
     <t>Low</t>
   </si>
   <si>
+    <t>Minor</t>
+  </si>
+  <si>
     <t>TC003</t>
   </si>
   <si>
@@ -227,13 +233,19 @@
   </si>
   <si>
     <t>Highest</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>Critical</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -367,6 +379,18 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -710,9 +734,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1088,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500B0826-BDED-8C4B-820B-BA9B03BB1156}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1106,7 +1132,7 @@
     <col min="17" max="17" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1158,734 +1184,765 @@
       <c r="Q1" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O2">
         <v>20</v>
       </c>
+      <c r="R2" s="3"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H3" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O3">
         <v>20</v>
       </c>
       <c r="P3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q3" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H4" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O4">
         <v>20</v>
       </c>
       <c r="P4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q4" t="s">
+        <v>39</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H5" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O5">
         <v>20</v>
       </c>
+      <c r="R5" s="3"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G6" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H6" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O6">
         <v>20</v>
       </c>
       <c r="P6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q6" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H7" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O7">
         <v>20</v>
       </c>
+      <c r="R7" s="3"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H8" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O8">
         <v>20</v>
       </c>
+      <c r="R8" s="3"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H9" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O9">
         <v>20</v>
       </c>
       <c r="P9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q9" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H10" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O10">
         <v>20</v>
       </c>
+      <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H11" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O11">
         <v>20</v>
       </c>
+      <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G12" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H12" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O12">
         <v>20</v>
       </c>
       <c r="P12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q12" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D13">
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H13" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O13">
         <v>20</v>
       </c>
+      <c r="R13" s="3"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H14" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O14">
         <v>20</v>
       </c>
       <c r="P14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q14" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H15" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O15">
         <v>20</v>
       </c>
+      <c r="R15" s="3"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H16" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L16" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O16">
         <v>20</v>
       </c>
+      <c r="R16" s="3"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H17" s="1">
         <v>45909.416666666664</v>
       </c>
       <c r="I17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O17">
         <v>20</v>
       </c>
+      <c r="R17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>